<commit_message>
run tests in serial
</commit_message>
<xml_diff>
--- a/NetXLSX.Test/Mock/mock_spreadsheet.xlsx
+++ b/NetXLSX.Test/Mock/mock_spreadsheet.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanb\code\netxlsx\NetXLSX.Test\Mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA41F136-8408-41D8-A9B3-E39B5D37CB5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF106D-65F2-4522-939C-94DC9FA5DAA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24300" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{9D4DA47C-3E6D-4A95-B2F8-E066552747C2}"/>
+    <workbookView xWindow="-23955" yWindow="2445" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{9D4DA47C-3E6D-4A95-B2F8-E066552747C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Partial" sheetId="2" r:id="rId2"/>
+    <sheet name="Complete" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>String Property</t>
   </si>
@@ -432,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D263213-DC55-4B7A-B464-57FF0F685182}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -500,4 +502,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFF2716-12D0-4DAD-9B69-4E48AC4FE010}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75086F4E-FB97-4697-9478-503A79E894FD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>